<commit_message>
Lab 4 added additional metrics for analysis: acf max level and value
</commit_message>
<xml_diff>
--- a/RecognitionSystems/Lab4/Metrics.xlsx
+++ b/RecognitionSystems/Lab4/Metrics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1005" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="1455" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="79">
   <si>
     <t xml:space="preserve"> 462.25</t>
   </si>
@@ -218,6 +218,39 @@
   </si>
   <si>
     <t>skewness</t>
+  </si>
+  <si>
+    <t>ACF_max_lvl</t>
+  </si>
+  <si>
+    <t>ACF_max_val</t>
+  </si>
+  <si>
+    <t>1.00000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.88298</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.88457</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.88879</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.90232</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.92042</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.92486</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.90416</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.90701</t>
   </si>
 </sst>
 </file>
@@ -559,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,9 +610,11 @@
     <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -616,8 +651,14 @@
       <c r="L1" t="s">
         <v>67</v>
       </c>
+      <c r="M1" t="s">
+        <v>68</v>
+      </c>
+      <c r="N1" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -654,8 +695,14 @@
       <c r="L2" t="s">
         <v>6</v>
       </c>
+      <c r="M2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N2" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -692,8 +739,14 @@
       <c r="L3" t="s">
         <v>13</v>
       </c>
+      <c r="M3" t="s">
+        <v>70</v>
+      </c>
+      <c r="N3" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -730,8 +783,14 @@
       <c r="L4" t="s">
         <v>20</v>
       </c>
+      <c r="M4" t="s">
+        <v>70</v>
+      </c>
+      <c r="N4" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -768,8 +827,14 @@
       <c r="L5" t="s">
         <v>27</v>
       </c>
+      <c r="M5" t="s">
+        <v>70</v>
+      </c>
+      <c r="N5" t="s">
+        <v>74</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -806,8 +871,14 @@
       <c r="L6" t="s">
         <v>34</v>
       </c>
+      <c r="M6" t="s">
+        <v>70</v>
+      </c>
+      <c r="N6" t="s">
+        <v>75</v>
+      </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -844,8 +915,14 @@
       <c r="L7" t="s">
         <v>41</v>
       </c>
+      <c r="M7" t="s">
+        <v>70</v>
+      </c>
+      <c r="N7" t="s">
+        <v>76</v>
+      </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -882,8 +959,14 @@
       <c r="L8" t="s">
         <v>48</v>
       </c>
+      <c r="M8" t="s">
+        <v>70</v>
+      </c>
+      <c r="N8" t="s">
+        <v>77</v>
+      </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -919,6 +1002,12 @@
       </c>
       <c r="L9" t="s">
         <v>55</v>
+      </c>
+      <c r="M9" t="s">
+        <v>70</v>
+      </c>
+      <c r="N9" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lab4 updated signal metrics calculation with mirroring initial signal value
</commit_message>
<xml_diff>
--- a/RecognitionSystems/Lab4/Metrics.xlsx
+++ b/RecognitionSystems/Lab4/Metrics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1455" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="2355" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="95">
   <si>
     <t xml:space="preserve"> 462.25</t>
   </si>
@@ -22,168 +22,42 @@
     <t xml:space="preserve"> 150.06</t>
   </si>
   <si>
-    <t xml:space="preserve"> 38004.25</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3051.80</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 4.44522</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 4.37298</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.10109</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 380.25</t>
   </si>
   <si>
     <t xml:space="preserve"> 139.54</t>
   </si>
   <si>
-    <t xml:space="preserve"> 18696.75</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1639.95</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3.11479</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 11.00103</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.16984</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 1296.00</t>
   </si>
   <si>
     <t xml:space="preserve"> 280.56</t>
   </si>
   <si>
-    <t xml:space="preserve"> 196918.50</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 16160.62</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5.04455</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 6.37507</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.12929</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 529.00</t>
   </si>
   <si>
     <t xml:space="preserve"> 201.29</t>
   </si>
   <si>
-    <t xml:space="preserve"> 68661.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5557.22</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 4.19882</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5.69933</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.04899</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 2704.00</t>
   </si>
   <si>
-    <t xml:space="preserve"> 859.22</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 150296.75</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 13138.80</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 8.74477</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 7.77893</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.35371</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 992.25</t>
   </si>
   <si>
     <t xml:space="preserve"> 317.29</t>
   </si>
   <si>
-    <t xml:space="preserve"> 43081.25</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2879.36</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 4.67025</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 9.41546</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.06100</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 1764.00</t>
   </si>
   <si>
-    <t xml:space="preserve"> 570.02</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 375975.75</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 31959.02</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 6.94361</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5.60789</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.12723</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 961.00</t>
   </si>
   <si>
     <t xml:space="preserve"> 297.56</t>
   </si>
   <si>
-    <t xml:space="preserve"> 52696.50</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 4049.09</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5.19149</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5.31615</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -0.04376</t>
-  </si>
-  <si>
     <t>Class</t>
   </si>
   <si>
@@ -226,31 +100,205 @@
     <t>ACF_max_val</t>
   </si>
   <si>
-    <t>1.00000</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.88298</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.88457</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.88879</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.90232</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.92042</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.92486</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.90416</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.90701</t>
+    <t xml:space="preserve"> 42917.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3454.58</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3.34672</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8.74918</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.87521</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 19083.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1671.47</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2.23798</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 23.27582</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.86315</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 308269.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 25248.20</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4.47533</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7.55783</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.87818</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 133078.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10909.69</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4.13475</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6.10194</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.90100</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1004.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 295571.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 26049.91</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8.67267</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8.03936</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.91954</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 43451.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2905.73</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3.32609</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21.13135</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.91410</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 597.19</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 666613.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 54450.20</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6.53871</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6.18797</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.90339</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 80087.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6506.56</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4.53869</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8.91472</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.89457</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21756.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 67126155.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 26896.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 268745645.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 22801.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 134355414.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 22350.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 67148325.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 25440.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 67154747.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 28900.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 269102453.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 25281.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 67187799.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 32400.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 67397523.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.11199</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  1.00000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.23038</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.09632</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.05132</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.35575</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.08201</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.11444</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -0.06168</t>
   </si>
 </sst>
 </file>
@@ -592,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,56 +654,56 @@
     <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>58</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>59</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>60</v>
+        <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="G1" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="H1" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="I1" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="J1" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="K1" t="s">
-        <v>66</v>
+        <v>24</v>
       </c>
       <c r="L1" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="M1" t="s">
-        <v>68</v>
+        <v>26</v>
       </c>
       <c r="N1" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -678,28 +726,28 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="H2">
         <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="J2" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="K2" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="L2" t="s">
-        <v>6</v>
+        <v>86</v>
       </c>
       <c r="M2" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="N2" t="s">
-        <v>71</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -710,40 +758,40 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="H3">
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="J3" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="K3" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="L3" t="s">
-        <v>13</v>
+        <v>88</v>
       </c>
       <c r="M3" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="N3" t="s">
-        <v>72</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -754,40 +802,40 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="H4">
         <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="J4" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="K4" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="L4" t="s">
-        <v>20</v>
+        <v>89</v>
       </c>
       <c r="M4" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="N4" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -798,216 +846,568 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="D5">
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="H5">
         <v>2</v>
       </c>
       <c r="I5" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="J5" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="K5" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="L5" t="s">
-        <v>27</v>
+        <v>90</v>
       </c>
       <c r="M5" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="N5" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="D6">
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="H6">
         <v>2</v>
       </c>
       <c r="I6" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J6" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="K6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="L6" t="s">
-        <v>34</v>
+        <v>88</v>
       </c>
       <c r="M6" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="N6" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="H7">
         <v>2</v>
       </c>
       <c r="I7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L7" t="s">
-        <v>41</v>
+        <v>89</v>
       </c>
       <c r="M7" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="N7" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8" t="s">
+        <v>75</v>
+      </c>
+      <c r="H8">
+        <v>2</v>
+      </c>
+      <c r="I8" t="s">
         <v>44</v>
       </c>
-      <c r="H8">
-        <v>2</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>45</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>46</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
+        <v>90</v>
+      </c>
+      <c r="M8" t="s">
+        <v>87</v>
+      </c>
+      <c r="N8" t="s">
         <v>47</v>
-      </c>
-      <c r="L8" t="s">
-        <v>48</v>
-      </c>
-      <c r="M8" t="s">
-        <v>70</v>
-      </c>
-      <c r="N8" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>77</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" t="s">
+        <v>86</v>
+      </c>
+      <c r="M9" t="s">
+        <v>87</v>
+      </c>
+      <c r="N9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
         <v>49</v>
       </c>
-      <c r="D9">
+      <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="I10" t="s">
+        <v>50</v>
+      </c>
+      <c r="J10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K10" t="s">
+        <v>52</v>
+      </c>
+      <c r="L10" t="s">
+        <v>91</v>
+      </c>
+      <c r="M10" t="s">
+        <v>87</v>
+      </c>
+      <c r="N10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11">
         <v>3</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+      <c r="I11" t="s">
+        <v>55</v>
+      </c>
+      <c r="J11" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11" t="s">
+        <v>57</v>
+      </c>
+      <c r="L11" t="s">
+        <v>92</v>
+      </c>
+      <c r="M11" t="s">
+        <v>87</v>
+      </c>
+      <c r="N11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12" t="s">
+        <v>61</v>
+      </c>
+      <c r="J12" t="s">
+        <v>62</v>
+      </c>
+      <c r="K12" t="s">
+        <v>63</v>
+      </c>
+      <c r="L12" t="s">
+        <v>93</v>
+      </c>
+      <c r="M12" t="s">
+        <v>87</v>
+      </c>
+      <c r="N12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>65</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13" t="s">
+        <v>66</v>
+      </c>
+      <c r="J13" t="s">
+        <v>67</v>
+      </c>
+      <c r="K13" t="s">
+        <v>68</v>
+      </c>
+      <c r="L13" t="s">
+        <v>94</v>
+      </c>
+      <c r="M13" t="s">
+        <v>87</v>
+      </c>
+      <c r="N13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14" t="s">
+        <v>79</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="I14" t="s">
+        <v>55</v>
+      </c>
+      <c r="J14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K14" t="s">
+        <v>57</v>
+      </c>
+      <c r="L14" t="s">
+        <v>92</v>
+      </c>
+      <c r="M14" t="s">
+        <v>87</v>
+      </c>
+      <c r="N14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
+        <v>81</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+      <c r="I15" t="s">
+        <v>61</v>
+      </c>
+      <c r="J15" t="s">
+        <v>62</v>
+      </c>
+      <c r="K15" t="s">
+        <v>63</v>
+      </c>
+      <c r="L15" t="s">
+        <v>93</v>
+      </c>
+      <c r="M15" t="s">
+        <v>87</v>
+      </c>
+      <c r="N15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>83</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16" t="s">
+        <v>66</v>
+      </c>
+      <c r="J16" t="s">
+        <v>67</v>
+      </c>
+      <c r="K16" t="s">
+        <v>68</v>
+      </c>
+      <c r="L16" t="s">
+        <v>94</v>
+      </c>
+      <c r="M16" t="s">
+        <v>87</v>
+      </c>
+      <c r="N16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>85</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+      <c r="I17" t="s">
         <v>50</v>
       </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="J17" t="s">
         <v>51</v>
       </c>
-      <c r="H9">
-        <v>2</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="K17" t="s">
         <v>52</v>
       </c>
-      <c r="J9" t="s">
+      <c r="L17" t="s">
+        <v>91</v>
+      </c>
+      <c r="M17" t="s">
+        <v>87</v>
+      </c>
+      <c r="N17" t="s">
         <v>53</v>
-      </c>
-      <c r="K9" t="s">
-        <v>54</v>
-      </c>
-      <c r="L9" t="s">
-        <v>55</v>
-      </c>
-      <c r="M9" t="s">
-        <v>70</v>
-      </c>
-      <c r="N9" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>